<commit_message>
completed CLI w/ save to .txt
</commit_message>
<xml_diff>
--- a/PS3.xlsx
+++ b/PS3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\game_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A8A702-24B2-495C-A35E-685C46A56204}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20594FC-53A2-4537-B71D-3BD6823B27EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38BBB09C-4BBE-40C8-BD08-FEC042D1F6E6}"/>
+    <workbookView xWindow="4140" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{38BBB09C-4BBE-40C8-BD08-FEC042D1F6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Title</t>
   </si>
@@ -118,6 +118,45 @@
   </si>
   <si>
     <t>Ubisoft</t>
+  </si>
+  <si>
+    <t>Team Bondi</t>
+  </si>
+  <si>
+    <t>Rockstar Games</t>
+  </si>
+  <si>
+    <t>Borderlands: The Pre-Sequel</t>
+  </si>
+  <si>
+    <t>2k Games</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto V</t>
+  </si>
+  <si>
+    <t>2K Australia</t>
+  </si>
+  <si>
+    <t>Rockstar North</t>
+  </si>
+  <si>
+    <t>Rocksteady Studios</t>
+  </si>
+  <si>
+    <t>Warner Bros.</t>
+  </si>
+  <si>
+    <t>Monolith</t>
+  </si>
+  <si>
+    <t>Visceral Games</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Sucker Punch</t>
   </si>
 </sst>
 </file>
@@ -484,18 +523,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF41043F-D6A2-4485-AF80-63BB39FCF901}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="4" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,6 +626,12 @@
       <c r="C5">
         <v>2011</v>
       </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
@@ -612,29 +656,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>2011</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>2014</v>
+        <v>2011</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -642,13 +678,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>2011</v>
+        <v>2014</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -656,13 +698,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>2008</v>
+        <v>2011</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -670,13 +718,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>2009</v>
+        <v>2008</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -684,33 +738,103 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>2009</v>
       </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>2009</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>2011</v>
       </c>
-      <c r="F13" t="s">
-        <v>8</v>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>2014</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>2013</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>